<commit_message>
created histo pie chart
</commit_message>
<xml_diff>
--- a/Proposals/Spencer,Laura-Budget Proposal.xlsx
+++ b/Proposals/Spencer,Laura-Budget Proposal.xlsx
@@ -13,8 +13,8 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BC54B5F8-7D07-9748-9441-533AB2E4D49F}" mergeInterval="0" personalView="1" windowWidth="1678" windowHeight="527" tabRatio="500" activeSheetId="1"/>
     <customWorkbookView name="Laura Spencer - Personal View" guid="{9EA234CE-FC9A-774F-BE98-9137C5772B66}" mergeInterval="0" personalView="1" yWindow="86" windowWidth="1280" windowHeight="690" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BC54B5F8-7D07-9748-9441-533AB2E4D49F}" mergeInterval="0" personalView="1" windowWidth="1678" windowHeight="527" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>Student Meeting Fund Budget Worksheet</t>
   </si>
@@ -285,6 +285,24 @@
   </si>
   <si>
     <t>Las Vegas, NV</t>
+  </si>
+  <si>
+    <t>SAFS FINS</t>
+  </si>
+  <si>
+    <t>Student registration fee</t>
+  </si>
+  <si>
+    <t>Transit within Las Vegas</t>
+  </si>
+  <si>
+    <t>Airfare SEA &lt;-&gt; Las Vegas</t>
+  </si>
+  <si>
+    <t>Meals not provided by AA</t>
+  </si>
+  <si>
+    <t>Hotel during conference</t>
   </si>
 </sst>
 </file>
@@ -555,7 +573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -668,6 +686,18 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,27 +744,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -746,6 +755,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -776,17 +806,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" indent="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -810,14 +832,14 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B040EE61-AD06-8D4A-A59D-A8637F311E57}" diskRevisions="1" revisionId="24" version="2" protected="1">
-  <header guid="{0F5E0D11-38D2-7847-929F-13574457C4AE}" dateTime="2015-12-03T14:25:35" maxSheetId="3" userName="Microsoft Office User" r:id="rId6">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{72AC2C25-CDD6-7842-9BC9-122EE7523B07}" diskRevisions="1" revisionId="38" version="3" protected="1">
+  <header guid="{B040EE61-AD06-8D4A-A59D-A8637F311E57}" dateTime="2017-10-26T14:20:20" maxSheetId="3" userName="Laura Spencer" r:id="rId7" minRId="1" maxRId="24">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
-  <header guid="{B040EE61-AD06-8D4A-A59D-A8637F311E57}" dateTime="2017-10-26T14:20:20" maxSheetId="3" userName="Laura Spencer" r:id="rId7" minRId="1" maxRId="24">
+  <header guid="{72AC2C25-CDD6-7842-9BC9-122EE7523B07}" dateTime="2017-10-27T16:44:06" maxSheetId="3" userName="Laura Spencer" r:id="rId8" minRId="25" maxRId="38">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -826,9 +848,121 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcmt sheetId="1" cell="F10" guid="{12CCFCD6-BCFC-FA46-9750-F3758B8A2BAB}" author="Microsoft Office User" newLength="132"/>
+  <rcc rId="25" sId="1">
+    <oc r="C31">
+      <v>156</v>
+    </oc>
+    <nc r="C31">
+      <v>160</v>
+    </nc>
+  </rcc>
+  <rcc rId="26" sId="1">
+    <oc r="C36">
+      <v>496</v>
+    </oc>
+    <nc r="C36">
+      <v>500</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D31">
+    <dxf>
+      <alignment horizontal="right" readingOrder="0"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="27" sId="1">
+    <oc r="E25" t="inlineStr">
+      <is>
+        <t>US Aquaculture Society</t>
+      </is>
+    </oc>
+    <nc r="E25" t="inlineStr">
+      <is>
+        <t>SAFS FINS</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="28" sId="1">
+    <oc r="D31">
+      <v>400</v>
+    </oc>
+    <nc r="D31">
+      <v>375</v>
+    </nc>
+  </rcc>
+  <rcc rId="29" sId="1">
+    <oc r="D25">
+      <v>100</v>
+    </oc>
+    <nc r="D25">
+      <v>121</v>
+    </nc>
+  </rcc>
+  <rcc rId="30" sId="1">
+    <nc r="F11" t="inlineStr">
+      <is>
+        <t>Pending</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="31" sId="1">
+    <nc r="F25" t="inlineStr">
+      <is>
+        <t>Pending</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="32" sId="1">
+    <nc r="F31" t="inlineStr">
+      <is>
+        <t>Pending</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="33" sId="1">
+    <nc r="G11" t="inlineStr">
+      <is>
+        <t>Student registration fee</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="34" sId="1">
+    <nc r="G16" t="inlineStr">
+      <is>
+        <t>Transit within Las Vegas</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="35" sId="1">
+    <nc r="G13" t="inlineStr">
+      <is>
+        <t>Airfare SEA &lt;-&gt; Las Vegas</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="36" sId="1">
+    <nc r="G25" t="inlineStr">
+      <is>
+        <t>Meals not provided by AA</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="37" sId="1">
+    <oc r="G20">
+      <f>SUM(G13:G19)</f>
+    </oc>
+    <nc r="G20">
+      <f>SUM(G13:G19)</f>
+    </nc>
+  </rcc>
+  <rcc rId="38" sId="1">
+    <nc r="G31" t="inlineStr">
+      <is>
+        <t>Hotel during conference</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -1008,7 +1142,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
@@ -1267,7 +1401,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1278,7 +1412,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:G8"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1293,48 +1427,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" customHeight="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="21">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-    </row>
-    <row r="4" spans="1:7" ht="19">
-      <c r="A4" s="58" t="s">
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+    </row>
+    <row r="4" spans="1:7" ht="18">
+      <c r="A4" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-    </row>
-    <row r="5" spans="1:7" ht="19">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+    </row>
+    <row r="5" spans="1:7" ht="18">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1347,7 +1481,7 @@
       <c r="F5" s="40"/>
       <c r="G5" s="41"/>
     </row>
-    <row r="6" spans="1:7" ht="19">
+    <row r="6" spans="1:7" ht="18">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1494,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="41"/>
     </row>
-    <row r="7" spans="1:7" ht="19">
+    <row r="7" spans="1:7" ht="18">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -1373,7 +1507,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="41"/>
     </row>
-    <row r="8" spans="1:7" ht="19">
+    <row r="8" spans="1:7" ht="18">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -1386,7 +1520,7 @@
       <c r="F8" s="40"/>
       <c r="G8" s="41"/>
     </row>
-    <row r="9" spans="1:7" ht="19">
+    <row r="9" spans="1:7" ht="18">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1395,7 +1529,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="19">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="18">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -1432,21 +1566,25 @@
       <c r="E11" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:7" ht="19">
+      <c r="F11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18">
       <c r="A12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="55"/>
-    </row>
-    <row r="13" spans="1:7" ht="19">
+      <c r="B12" s="57"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+    </row>
+    <row r="13" spans="1:7" ht="36">
       <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
@@ -1457,9 +1595,11 @@
       <c r="D13" s="15"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" ht="19">
+      <c r="G13" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18">
       <c r="A14" s="14" t="s">
         <v>23</v>
       </c>
@@ -1470,7 +1610,7 @@
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
     </row>
-    <row r="15" spans="1:7" ht="19">
+    <row r="15" spans="1:7" ht="18">
       <c r="A15" s="14" t="s">
         <v>24</v>
       </c>
@@ -1481,7 +1621,7 @@
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
     </row>
-    <row r="16" spans="1:7" ht="19">
+    <row r="16" spans="1:7" ht="18">
       <c r="A16" s="14" t="s">
         <v>25</v>
       </c>
@@ -1492,9 +1632,11 @@
       <c r="D16" s="15"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-    </row>
-    <row r="17" spans="1:7" ht="19">
+      <c r="G16" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18">
       <c r="A17" s="14" t="s">
         <v>19</v>
       </c>
@@ -1505,7 +1647,7 @@
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
     </row>
-    <row r="18" spans="1:7" ht="19">
+    <row r="18" spans="1:7" ht="18">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -1516,7 +1658,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" ht="19">
+    <row r="19" spans="1:7" ht="18">
       <c r="A19" s="14" t="s">
         <v>6</v>
       </c>
@@ -1527,7 +1669,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
     </row>
-    <row r="20" spans="1:7" ht="19">
+    <row r="20" spans="1:7" ht="18">
       <c r="A20" s="10" t="s">
         <v>29</v>
       </c>
@@ -1551,61 +1693,61 @@
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(G13:G19)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19">
+    <row r="21" spans="1:7" ht="18">
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
-    </row>
-    <row r="22" spans="1:7" ht="19">
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="59"/>
+    </row>
+    <row r="22" spans="1:7" ht="18">
       <c r="A22" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="8">
         <v>64</v>
       </c>
-      <c r="C22" s="45"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="47"/>
-    </row>
-    <row r="23" spans="1:7" ht="19">
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="51"/>
+    </row>
+    <row r="23" spans="1:7" ht="18">
       <c r="A23" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="8">
         <v>25</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="47"/>
-    </row>
-    <row r="24" spans="1:7" ht="19">
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+    </row>
+    <row r="24" spans="1:7" ht="18">
       <c r="A24" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="8">
         <v>4</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-    </row>
-    <row r="25" spans="1:7" ht="18">
+      <c r="C24" s="52"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="54"/>
+    </row>
+    <row r="25" spans="1:7" ht="36">
       <c r="A25" s="10" t="s">
         <v>10</v>
       </c>
@@ -1615,76 +1757,80 @@
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" ht="19">
+        <v>59</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18">
       <c r="A26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="55"/>
-    </row>
-    <row r="27" spans="1:7" ht="19">
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="59"/>
+    </row>
+    <row r="27" spans="1:7" ht="18">
       <c r="A27" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="8">
         <v>134</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
-    </row>
-    <row r="28" spans="1:7" ht="19">
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+    </row>
+    <row r="28" spans="1:7" ht="18">
       <c r="A28" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="8">
         <v>139</v>
       </c>
-      <c r="C28" s="45"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="47"/>
-    </row>
-    <row r="29" spans="1:7" ht="19">
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="51"/>
+    </row>
+    <row r="29" spans="1:7" ht="18">
       <c r="A29" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="8">
         <v>4</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="47"/>
-    </row>
-    <row r="30" spans="1:7" ht="19">
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="51"/>
+    </row>
+    <row r="30" spans="1:7" ht="18">
       <c r="A30" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="8">
         <v>1</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="54"/>
     </row>
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="9" t="s">
@@ -1695,18 +1841,22 @@
         <v>556</v>
       </c>
       <c r="C31" s="17">
-        <v>156</v>
-      </c>
-      <c r="D31" s="18">
-        <v>400</v>
+        <v>160</v>
+      </c>
+      <c r="D31" s="80">
+        <v>375</v>
       </c>
       <c r="E31" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="19">
+      <c r="F31" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18">
       <c r="A32" s="3" t="s">
         <v>26</v>
       </c>
@@ -1718,25 +1868,25 @@
       <c r="G32" s="21"/>
     </row>
     <row r="33" spans="1:7" ht="19" customHeight="1">
-      <c r="A33" s="51"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
+      <c r="A33" s="55"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
     </row>
     <row r="34" spans="1:7" ht="19" customHeight="1">
-      <c r="A34" s="52"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-    </row>
-    <row r="35" spans="1:7" ht="19">
-      <c r="A35" s="42"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="56"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+    </row>
+    <row r="35" spans="1:7" ht="18">
+      <c r="A35" s="46"/>
       <c r="B35" s="3" t="s">
         <v>16</v>
       </c>
@@ -1752,20 +1902,20 @@
       <c r="F35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="44"/>
-    </row>
-    <row r="36" spans="1:7" ht="19">
-      <c r="A36" s="42"/>
+      <c r="G35" s="48"/>
+    </row>
+    <row r="36" spans="1:7" ht="18">
+      <c r="A36" s="46"/>
       <c r="B36" s="4">
         <f>SUM(B11+B20+B25+B31+B32)</f>
         <v>1221</v>
       </c>
       <c r="C36" s="4">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="D36" s="4">
         <f>(D11+D20+D25+D31+D32)</f>
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="E36" s="4">
         <f>C36+D36</f>
@@ -1775,25 +1925,25 @@
         <f>B36-E36</f>
         <v>0</v>
       </c>
-      <c r="G36" s="44"/>
+      <c r="G36" s="48"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="43"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="43"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="43"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
     </row>
     <row r="39" spans="1:7">
       <c r="C39" s="1"/>
@@ -1806,6 +1956,13 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BC54B5F8-7D07-9748-9441-533AB2E4D49F}" showRuler="0" topLeftCell="A3">
+      <selection activeCell="E10" sqref="E10"/>
+      <colBreaks count="1" manualBreakCount="1">
+        <brk id="7" max="1048575" man="1"/>
+      </colBreaks>
+      <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+    </customSheetView>
     <customSheetView guid="{9EA234CE-FC9A-774F-BE98-9137C5772B66}" showRuler="0">
       <selection activeCell="B8" sqref="B8:G8"/>
       <colBreaks count="1" manualBreakCount="1">
@@ -1813,20 +1970,8 @@
       </colBreaks>
       <pageSetup scale="47" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{BC54B5F8-7D07-9748-9441-533AB2E4D49F}" showRuler="0" topLeftCell="A3">
-      <selection activeCell="E10" sqref="E10"/>
-      <colBreaks count="1" manualBreakCount="1">
-        <brk id="7" max="1048575" man="1"/>
-      </colBreaks>
-      <pageSetup scale="47" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-    </customSheetView>
   </customSheetViews>
   <mergeCells count="16">
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A4:G4"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="A35:A36"/>
@@ -1838,6 +1983,11 @@
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A4:G4"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
@@ -1851,7 +2001,7 @@
     <hyperlink ref="A18" r:id="rId8"/>
     <hyperlink ref="A19" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="47" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="7" max="1048575" man="1"/>
@@ -1885,100 +2035,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" customHeight="1">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
     </row>
     <row r="2" spans="1:7" ht="16" customHeight="1">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1" ht="21">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-    </row>
-    <row r="4" spans="1:7" ht="19">
-      <c r="A4" s="78" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+    </row>
+    <row r="4" spans="1:7" ht="18">
+      <c r="A4" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-    </row>
-    <row r="5" spans="1:7" ht="19">
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+    </row>
+    <row r="5" spans="1:7" ht="18">
       <c r="A5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="G5" s="65"/>
-    </row>
-    <row r="6" spans="1:7" ht="19">
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
+    </row>
+    <row r="6" spans="1:7" ht="18">
       <c r="A6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="65"/>
-    </row>
-    <row r="7" spans="1:7" ht="19">
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
+    </row>
+    <row r="7" spans="1:7" ht="18">
       <c r="A7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="65"/>
-    </row>
-    <row r="8" spans="1:7" ht="19">
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+    </row>
+    <row r="8" spans="1:7" ht="18">
       <c r="A8" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="65"/>
-    </row>
-    <row r="9" spans="1:7" ht="19">
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+    </row>
+    <row r="9" spans="1:7" ht="18">
       <c r="A9" s="23"/>
       <c r="B9" s="24"/>
       <c r="C9" s="24"/>
@@ -1987,7 +2137,7 @@
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="19">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="18">
       <c r="A10" s="22" t="s">
         <v>18</v>
       </c>
@@ -2010,7 +2160,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="19">
+    <row r="11" spans="1:7" ht="18">
       <c r="A11" s="25" t="s">
         <v>3</v>
       </c>
@@ -2033,18 +2183,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="19">
+    <row r="12" spans="1:7" ht="18">
       <c r="A12" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="68"/>
-    </row>
-    <row r="13" spans="1:7" ht="38">
+      <c r="B12" s="70"/>
+      <c r="C12" s="71"/>
+      <c r="D12" s="71"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
+    </row>
+    <row r="13" spans="1:7" ht="36">
       <c r="A13" s="30" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2217,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="19">
+    <row r="14" spans="1:7" ht="18">
       <c r="A14" s="30" t="s">
         <v>23</v>
       </c>
@@ -2080,7 +2230,7 @@
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
     </row>
-    <row r="15" spans="1:7" ht="19">
+    <row r="15" spans="1:7" ht="18">
       <c r="A15" s="30" t="s">
         <v>24</v>
       </c>
@@ -2093,7 +2243,7 @@
       <c r="F15" s="33"/>
       <c r="G15" s="33"/>
     </row>
-    <row r="16" spans="1:7" ht="38">
+    <row r="16" spans="1:7" ht="36">
       <c r="A16" s="30" t="s">
         <v>25</v>
       </c>
@@ -2116,7 +2266,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="19">
+    <row r="17" spans="1:7" ht="18">
       <c r="A17" s="30" t="s">
         <v>19</v>
       </c>
@@ -2129,7 +2279,7 @@
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
     </row>
-    <row r="18" spans="1:7" ht="19">
+    <row r="18" spans="1:7" ht="18">
       <c r="A18" s="30" t="s">
         <v>5</v>
       </c>
@@ -2142,7 +2292,7 @@
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
     </row>
-    <row r="19" spans="1:7" ht="19">
+    <row r="19" spans="1:7" ht="18">
       <c r="A19" s="30" t="s">
         <v>6</v>
       </c>
@@ -2155,7 +2305,7 @@
       <c r="F19" s="33"/>
       <c r="G19" s="33"/>
     </row>
-    <row r="20" spans="1:7" ht="19">
+    <row r="20" spans="1:7" ht="18">
       <c r="A20" s="25" t="s">
         <v>29</v>
       </c>
@@ -2184,57 +2334,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="19">
+    <row r="21" spans="1:7" ht="18">
       <c r="A21" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="68"/>
-    </row>
-    <row r="22" spans="1:7" ht="19">
+      <c r="B21" s="70"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="72"/>
+    </row>
+    <row r="22" spans="1:7" ht="18">
       <c r="A22" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="31">
         <v>74</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="70"/>
-    </row>
-    <row r="23" spans="1:7" ht="19">
+      <c r="C22" s="68"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
+    </row>
+    <row r="23" spans="1:7" ht="18">
       <c r="A23" s="35" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="31">
         <v>53</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="70"/>
-    </row>
-    <row r="24" spans="1:7" ht="19">
+      <c r="C23" s="68"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="74"/>
+    </row>
+    <row r="24" spans="1:7" ht="18">
       <c r="A24" s="35" t="s">
         <v>9</v>
       </c>
       <c r="B24" s="31">
         <v>6</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="73"/>
-    </row>
-    <row r="25" spans="1:7" ht="19">
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="77"/>
+    </row>
+    <row r="25" spans="1:7" ht="18">
       <c r="A25" s="25" t="s">
         <v>10</v>
       </c>
@@ -2256,70 +2406,70 @@
       </c>
       <c r="G25" s="37"/>
     </row>
-    <row r="26" spans="1:7" ht="19">
+    <row r="26" spans="1:7" ht="18">
       <c r="A26" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="68"/>
-    </row>
-    <row r="27" spans="1:7" ht="19">
+      <c r="B26" s="70"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="72"/>
+    </row>
+    <row r="27" spans="1:7" ht="18">
       <c r="A27" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="31">
         <v>250</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="70"/>
-    </row>
-    <row r="28" spans="1:7" ht="19">
+      <c r="C27" s="68"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="74"/>
+    </row>
+    <row r="28" spans="1:7" ht="18">
       <c r="A28" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="31">
         <v>175</v>
       </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="70"/>
-    </row>
-    <row r="29" spans="1:7" ht="19">
+      <c r="C28" s="68"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="74"/>
+    </row>
+    <row r="29" spans="1:7" ht="18">
       <c r="A29" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="31">
         <v>5</v>
       </c>
-      <c r="C29" s="61"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="70"/>
-    </row>
-    <row r="30" spans="1:7" ht="19">
+      <c r="C29" s="68"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="74"/>
+    </row>
+    <row r="30" spans="1:7" ht="18">
       <c r="A30" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="31">
         <v>2</v>
       </c>
-      <c r="C30" s="71"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
-    </row>
-    <row r="31" spans="1:7" ht="76">
+      <c r="C30" s="75"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="77"/>
+    </row>
+    <row r="31" spans="1:7" ht="72">
       <c r="A31" s="38" t="s">
         <v>15</v>
       </c>
@@ -2343,7 +2493,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="19">
+    <row r="32" spans="1:7" ht="18">
       <c r="A32" s="22" t="s">
         <v>26</v>
       </c>
@@ -2357,25 +2507,25 @@
       <c r="G32" s="37"/>
     </row>
     <row r="33" spans="1:7" ht="19" customHeight="1">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
     </row>
     <row r="34" spans="1:7" ht="19" customHeight="1">
-      <c r="A34" s="75"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-    </row>
-    <row r="35" spans="1:7" ht="19">
-      <c r="A35" s="60"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="79"/>
+    </row>
+    <row r="35" spans="1:7" ht="18">
+      <c r="A35" s="67"/>
       <c r="B35" s="22" t="s">
         <v>16</v>
       </c>
@@ -2391,10 +2541,10 @@
       <c r="F35" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G35" s="61"/>
-    </row>
-    <row r="36" spans="1:7" ht="19">
-      <c r="A36" s="60"/>
+      <c r="G35" s="68"/>
+    </row>
+    <row r="36" spans="1:7" ht="18">
+      <c r="A36" s="67"/>
       <c r="B36" s="31">
         <f>SUM(B11+B20+B25+B31+B32)</f>
         <v>1225.5</v>
@@ -2415,25 +2565,25 @@
         <f>B36-E36</f>
         <v>0</v>
       </c>
-      <c r="G36" s="61"/>
+      <c r="G36" s="68"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="62"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="62"/>
+      <c r="A37" s="69"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="62"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="62"/>
+      <c r="A38" s="69"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
     </row>
     <row r="39" spans="1:7">
       <c r="C39" s="1"/>
@@ -2446,20 +2596,14 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9EA234CE-FC9A-774F-BE98-9137C5772B66}" showRuler="0" topLeftCell="A25">
+    <customSheetView guid="{BC54B5F8-7D07-9748-9441-533AB2E4D49F}" showRuler="0" topLeftCell="A25">
       <selection activeCell="D47" sqref="D47"/>
     </customSheetView>
-    <customSheetView guid="{BC54B5F8-7D07-9748-9441-533AB2E4D49F}" showRuler="0" topLeftCell="A25">
+    <customSheetView guid="{9EA234CE-FC9A-774F-BE98-9137C5772B66}" showRuler="0" topLeftCell="A25">
       <selection activeCell="D47" sqref="D47"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="16">
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="G35:G36"/>
     <mergeCell ref="A37:G38"/>
@@ -2470,6 +2614,12 @@
     <mergeCell ref="B26:G26"/>
     <mergeCell ref="C27:G30"/>
     <mergeCell ref="A33:G34"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A27" r:id="rId1"/>
@@ -2482,7 +2632,7 @@
     <hyperlink ref="A18" r:id="rId8"/>
     <hyperlink ref="A19" r:id="rId9"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>